<commit_message>
added normalization in GrowthMovpe2
</commit_message>
<xml_diff>
--- a/IKZ_plugin/tests/data/movpe_IKZ/movpe2_growth_parser/GaO.growth.movpe.ikz.xlsx
+++ b/IKZ_plugin/tests/data/movpe_IKZ/movpe2_growth_parser/GaO.growth.movpe.ikz.xlsx
@@ -841,8 +841,8 @@
   </sheetPr>
   <dimension ref="A1:ALT14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AK20" activeCellId="0" sqref="AK20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5649,7 +5649,7 @@
         <v>83</v>
       </c>
       <c r="B13" s="42" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>80</v>
@@ -6735,7 +6735,7 @@
         <v>84</v>
       </c>
       <c r="B14" s="42" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C14" s="42" t="s">
         <v>85</v>

</xml_diff>